<commit_message>
Pushing the Test file for second time
</commit_message>
<xml_diff>
--- a/Test.xlsx
+++ b/Test.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\S787296\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\S787296\Documents\kirthi-git\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -35,10 +35,10 @@
     <t>Comments</t>
   </si>
   <si>
-    <t>PASS</t>
+    <t>Done</t>
   </si>
   <si>
-    <t>Done</t>
+    <t>FAIL</t>
   </si>
 </sst>
 </file>
@@ -375,7 +375,7 @@
   <dimension ref="A1:C11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+      <selection activeCell="B3" sqref="B2:B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -399,10 +399,10 @@
         <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -410,10 +410,10 @@
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
@@ -421,10 +421,10 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
@@ -432,10 +432,10 @@
         <v>4</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
@@ -443,10 +443,10 @@
         <v>5</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
@@ -454,10 +454,10 @@
         <v>6</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
@@ -465,10 +465,10 @@
         <v>7</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
@@ -476,10 +476,10 @@
         <v>8</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
@@ -487,10 +487,10 @@
         <v>9</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
@@ -498,10 +498,10 @@
         <v>10</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>